<commit_message>
couldnt find a way to nest the 3 dfs in pandas dataclass, so created one with school, teacher as index
</commit_message>
<xml_diff>
--- a/example_dataset.xlsx
+++ b/example_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ccaekbu_ucl_ac_uk/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{92C3C31E-B11F-41AE-964C-34B1FBB2BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B635703-EB3B-453E-A320-0FA62C635A4C}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{92C3C31E-B11F-41AE-964C-34B1FBB2BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A32E7D0-36E1-4427-B3B0-D5E23592F1A6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F5F4F09-FFBF-FF42-8606-4D2782A9E922}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="208">
   <si>
     <t>reg_rr_title</t>
   </si>
@@ -605,27 +605,6 @@
     <t>J School</t>
   </si>
   <si>
-    <t>RRS10800XX</t>
-  </si>
-  <si>
-    <t>RRS20302XX</t>
-  </si>
-  <si>
-    <t>RRS20100XX</t>
-  </si>
-  <si>
-    <t>RRS20200XX</t>
-  </si>
-  <si>
-    <t>RRS20705XX</t>
-  </si>
-  <si>
-    <t>RRS20104XX</t>
-  </si>
-  <si>
-    <t>RRS20701XX</t>
-  </si>
-  <si>
     <t>AB098XX</t>
   </si>
   <si>
@@ -654,6 +633,36 @@
   </si>
   <si>
     <t>AF055XX</t>
+  </si>
+  <si>
+    <t>RRS1080080</t>
+  </si>
+  <si>
+    <t>RRS2030220</t>
+  </si>
+  <si>
+    <t>RRS2010080</t>
+  </si>
+  <si>
+    <t>RRS4030010</t>
+  </si>
+  <si>
+    <t>RRS2020030</t>
+  </si>
+  <si>
+    <t>RRS2070510</t>
+  </si>
+  <si>
+    <t>RRS2020080</t>
+  </si>
+  <si>
+    <t>RRS2010450</t>
+  </si>
+  <si>
+    <t>RRS2070140</t>
+  </si>
+  <si>
+    <t>RRS2030250</t>
   </si>
 </sst>
 </file>
@@ -661,7 +670,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -710,8 +719,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1033,7 +1042,7 @@
   <dimension ref="A1:BR34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BK17" sqref="BK17"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1261,7 +1270,7 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -1276,7 +1285,7 @@
         <v>178</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="H2" t="s">
         <v>69</v>
@@ -1470,7 +1479,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
         <v>68</v>
@@ -1485,7 +1494,7 @@
         <v>178</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="H3" t="s">
         <v>69</v>
@@ -1679,7 +1688,7 @@
         <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
         <v>81</v>
@@ -1694,7 +1703,7 @@
         <v>179</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="H4" t="s">
         <v>69</v>
@@ -1888,7 +1897,7 @@
         <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>81</v>
@@ -1903,7 +1912,7 @@
         <v>179</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="H5" t="s">
         <v>69</v>
@@ -2097,7 +2106,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
         <v>81</v>
@@ -2112,7 +2121,7 @@
         <v>179</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="H6" t="s">
         <v>69</v>
@@ -2309,7 +2318,7 @@
         <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
@@ -2324,7 +2333,7 @@
         <v>179</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="H7" t="s">
         <v>69</v>
@@ -2518,7 +2527,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C8" t="s">
         <v>81</v>
@@ -2533,7 +2542,7 @@
         <v>180</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="H8" t="s">
         <v>69</v>
@@ -2727,7 +2736,7 @@
         <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C9" t="s">
         <v>68</v>
@@ -2742,7 +2751,7 @@
         <v>181</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="H9" t="s">
         <v>69</v>
@@ -2936,7 +2945,7 @@
         <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
@@ -2951,7 +2960,7 @@
         <v>181</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="H10" t="s">
         <v>69</v>
@@ -3145,7 +3154,7 @@
         <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C11" t="s">
         <v>68</v>
@@ -3160,7 +3169,7 @@
         <v>181</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="H11" t="s">
         <v>69</v>
@@ -3354,7 +3363,7 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C12" t="s">
         <v>68</v>
@@ -3369,7 +3378,7 @@
         <v>181</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="H12" t="s">
         <v>69</v>
@@ -3563,7 +3572,7 @@
         <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C13" t="s">
         <v>140</v>
@@ -3578,7 +3587,7 @@
         <v>182</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="H13" t="s">
         <v>69</v>
@@ -3772,7 +3781,7 @@
         <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C14" t="s">
         <v>140</v>
@@ -3787,7 +3796,7 @@
         <v>182</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="H14" t="s">
         <v>69</v>
@@ -3981,7 +3990,7 @@
         <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
         <v>140</v>
@@ -3996,7 +4005,7 @@
         <v>182</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="H15" t="s">
         <v>69</v>
@@ -4190,7 +4199,7 @@
         <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="C16" t="s">
         <v>140</v>
@@ -4205,7 +4214,7 @@
         <v>182</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="H16" t="s">
         <v>69</v>
@@ -4399,7 +4408,7 @@
         <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C17" t="s">
         <v>81</v>
@@ -4414,7 +4423,7 @@
         <v>183</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="H17" t="s">
         <v>69</v>
@@ -4608,7 +4617,7 @@
         <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
         <v>81</v>
@@ -4623,7 +4632,7 @@
         <v>183</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="H18" t="s">
         <v>69</v>
@@ -4817,7 +4826,7 @@
         <v>105</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
         <v>81</v>
@@ -4832,7 +4841,7 @@
         <v>183</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="H19" t="s">
         <v>69</v>
@@ -5026,7 +5035,7 @@
         <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C20" t="s">
         <v>81</v>
@@ -5041,7 +5050,7 @@
         <v>183</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="H20" t="s">
         <v>69</v>
@@ -5238,7 +5247,7 @@
         <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C21" t="s">
         <v>81</v>
@@ -5253,7 +5262,7 @@
         <v>184</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="H21" t="s">
         <v>69</v>
@@ -5447,7 +5456,7 @@
         <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C22" t="s">
         <v>81</v>
@@ -5462,7 +5471,7 @@
         <v>184</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="H22" t="s">
         <v>69</v>
@@ -5656,7 +5665,7 @@
         <v>105</v>
       </c>
       <c r="B23" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C23" t="s">
         <v>81</v>
@@ -5671,7 +5680,7 @@
         <v>184</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="H23" t="s">
         <v>69</v>
@@ -5865,7 +5874,7 @@
         <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C24" t="s">
         <v>81</v>
@@ -5880,7 +5889,7 @@
         <v>185</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="H24" t="s">
         <v>69</v>
@@ -6074,7 +6083,7 @@
         <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C25" t="s">
         <v>81</v>
@@ -6089,7 +6098,7 @@
         <v>185</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
       <c r="H25" t="s">
         <v>69</v>
@@ -6283,7 +6292,7 @@
         <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C26" t="s">
         <v>81</v>
@@ -6298,7 +6307,7 @@
         <v>186</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="H26" t="s">
         <v>69</v>
@@ -6492,7 +6501,7 @@
         <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
         <v>81</v>
@@ -6507,7 +6516,7 @@
         <v>186</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="H27" t="s">
         <v>69</v>
@@ -6701,7 +6710,7 @@
         <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C28" t="s">
         <v>81</v>
@@ -6716,7 +6725,7 @@
         <v>186</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="H28" t="s">
         <v>69</v>
@@ -6910,7 +6919,7 @@
         <v>111</v>
       </c>
       <c r="B29" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
         <v>81</v>
@@ -6925,7 +6934,7 @@
         <v>186</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="H29" t="s">
         <v>69</v>
@@ -7119,7 +7128,7 @@
         <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C30" t="s">
         <v>81</v>
@@ -7134,7 +7143,7 @@
         <v>187</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H30" t="s">
         <v>69</v>
@@ -7328,7 +7337,7 @@
         <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C31" t="s">
         <v>81</v>
@@ -7343,7 +7352,7 @@
         <v>187</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H31" t="s">
         <v>69</v>
@@ -7537,7 +7546,7 @@
         <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C32" t="s">
         <v>81</v>
@@ -7552,7 +7561,7 @@
         <v>187</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H32" t="s">
         <v>69</v>
@@ -7746,7 +7755,7 @@
         <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C33" t="s">
         <v>81</v>
@@ -7761,7 +7770,7 @@
         <v>187</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H33" t="s">
         <v>69</v>
@@ -7958,7 +7967,7 @@
         <v>174</v>
       </c>
       <c r="B34" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C34" t="s">
         <v>81</v>
@@ -7973,7 +7982,7 @@
         <v>187</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="H34" t="s">
         <v>69</v>

</xml_diff>